<commit_message>
added new column data
</commit_message>
<xml_diff>
--- a/ImportantFile.xlsx
+++ b/ImportantFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Santosh\SantoshTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE682B59-7E09-416D-A436-F37CBD866D08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528F2218-8D47-472D-B59F-DBFC3D7D8A69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Name</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>Peter</t>
+  </si>
+  <si>
+    <t>Dept</t>
+  </si>
+  <si>
+    <t>AP</t>
   </si>
 </sst>
 </file>
@@ -351,28 +357,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>